<commit_message>
1. Fix Month 0 Evolution Bug 2. Redistribute Contributions When Category Empty 3. Add BEP.UN to Category Set 4. Add Input Validation 5. Add Division by Zero Guard
</commit_message>
<xml_diff>
--- a/projection_output/portfolio_10yr_realistic_summary.xlsx
+++ b/projection_output/portfolio_10yr_realistic_summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/affa4e204ffd6129/GitClone/InvestmentModeling/projection_output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/affa4e204ffd6129/GitClone/InvestmentModelling/projection_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_424DA3359E9199DADF55C072FCF2D3C204DD71E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6869B653-0650-453E-B26D-E2E1B5BF3589}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_841861279E9199DADF55C072FCF2D3C2045FCCD0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{920F5E1E-316F-4471-B2C8-D9E6661CFF61}"/>
   <bookViews>
-    <workbookView xWindow="9285" yWindow="1410" windowWidth="38700" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9975" yWindow="2100" windowWidth="38700" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,6 +54,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -90,16 +100,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,16 +418,17 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -435,139 +449,139 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1000</v>
       </c>
-      <c r="B2">
-        <v>413838.96529589623</v>
-      </c>
-      <c r="C2">
-        <v>30721.125519792869</v>
-      </c>
-      <c r="D2">
-        <v>339492.09160258173</v>
-      </c>
-      <c r="E2">
-        <v>25202.023090413331</v>
+      <c r="B2" s="2">
+        <v>413274.62897982268</v>
+      </c>
+      <c r="C2" s="2">
+        <v>30553.772961806899</v>
+      </c>
+      <c r="D2" s="2">
+        <v>339029.13926513313</v>
+      </c>
+      <c r="E2" s="2">
+        <v>25064.73570398978</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>1500</v>
       </c>
-      <c r="B3">
-        <v>523143.36077825108</v>
-      </c>
-      <c r="C3">
-        <v>37714.549154967834</v>
-      </c>
-      <c r="D3">
-        <v>429159.76660541329</v>
-      </c>
-      <c r="E3">
-        <v>30939.066279835821</v>
+      <c r="B3" s="2">
+        <v>523563.0729180249</v>
+      </c>
+      <c r="C3" s="2">
+        <v>37774.158789359877</v>
+      </c>
+      <c r="D3" s="2">
+        <v>429504.0767457136</v>
+      </c>
+      <c r="E3" s="2">
+        <v>30987.96694206553</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>2000</v>
       </c>
-      <c r="B4">
-        <v>621128.32346204878</v>
-      </c>
-      <c r="C4">
-        <v>41325.231718985109</v>
-      </c>
-      <c r="D4">
-        <v>509541.56415639719</v>
-      </c>
-      <c r="E4">
-        <v>33901.083582616273</v>
+      <c r="B4" s="2">
+        <v>622061.2902191258</v>
+      </c>
+      <c r="C4" s="2">
+        <v>41167.014828503197</v>
+      </c>
+      <c r="D4" s="2">
+        <v>510306.92184940551</v>
+      </c>
+      <c r="E4" s="2">
+        <v>33771.29062549791</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>2500</v>
       </c>
-      <c r="B5">
-        <v>733533.14270805311</v>
-      </c>
-      <c r="C5">
-        <v>48754.74479323667</v>
-      </c>
-      <c r="D5">
-        <v>601752.66652263107</v>
-      </c>
-      <c r="E5">
-        <v>39995.872001978772</v>
+      <c r="B5" s="2">
+        <v>737269.80480622686</v>
+      </c>
+      <c r="C5" s="2">
+        <v>49659.178289565563</v>
+      </c>
+      <c r="D5" s="2">
+        <v>604818.03092207585</v>
+      </c>
+      <c r="E5" s="2">
+        <v>40737.822483042313</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>3000</v>
       </c>
-      <c r="B6">
-        <v>845918.28321432264</v>
-      </c>
-      <c r="C6">
-        <v>56754.067359042572</v>
-      </c>
-      <c r="D6">
-        <v>693947.62546817958</v>
-      </c>
-      <c r="E6">
-        <v>46558.102668990607</v>
+      <c r="B6" s="2">
+        <v>845897.35236389283</v>
+      </c>
+      <c r="C6" s="2">
+        <v>56314.778021926068</v>
+      </c>
+      <c r="D6" s="2">
+        <v>693930.45488061442</v>
+      </c>
+      <c r="E6" s="2">
+        <v>46197.732408133808</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>3500</v>
       </c>
-      <c r="B7">
-        <v>949970.31793686654</v>
-      </c>
-      <c r="C7">
-        <v>61762.672757952387</v>
-      </c>
-      <c r="D7">
-        <v>779306.53525136912</v>
-      </c>
-      <c r="E7">
-        <v>50666.903592731796</v>
+      <c r="B7" s="2">
+        <v>951852.76737273403</v>
+      </c>
+      <c r="C7" s="2">
+        <v>61534.393198757527</v>
+      </c>
+      <c r="D7" s="2">
+        <v>780850.79944568395</v>
+      </c>
+      <c r="E7" s="2">
+        <v>50479.634844450047</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>4000</v>
       </c>
-      <c r="B8">
-        <v>1057180.515880022</v>
-      </c>
-      <c r="C8">
-        <v>68961.793868628229</v>
-      </c>
-      <c r="D8">
-        <v>867256.23886331567</v>
-      </c>
-      <c r="E8">
-        <v>56572.690356470062</v>
+      <c r="B8" s="2">
+        <v>1060396.689416847</v>
+      </c>
+      <c r="C8" s="2">
+        <v>68923.707077803323</v>
+      </c>
+      <c r="D8" s="2">
+        <v>869894.62135635363</v>
+      </c>
+      <c r="E8" s="2">
+        <v>56541.445922369159</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>5000</v>
       </c>
-      <c r="B9">
-        <v>1272514.4014187609</v>
-      </c>
-      <c r="C9">
-        <v>79797.32272507844</v>
-      </c>
-      <c r="D9">
-        <v>1043905.025770532</v>
-      </c>
-      <c r="E9">
-        <v>65461.598032107169</v>
+      <c r="B9" s="2">
+        <v>1279712.4929762781</v>
+      </c>
+      <c r="C9" s="2">
+        <v>81115.775720868696</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1049809.967942086</v>
+      </c>
+      <c r="E9" s="2">
+        <v>66543.188705669018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>